<commit_message>
part 2 completes (fix r problem and create a dataset)
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52.72758786833</v>
+        <v>71.66704759788001</v>
       </c>
       <c r="C2" t="n">
-        <v>72.89732575280001</v>
+        <v>95.96322044903999</v>
       </c>
       <c r="D2" t="n">
-        <v>63.69652859903</v>
+        <v>84.28312065108</v>
       </c>
       <c r="E2" t="n">
-        <v>4052.52265974881</v>
+        <v>5605.17276423382</v>
       </c>
       <c r="F2" t="n">
-        <v>5658.25050841565</v>
+        <v>7739.434472504409</v>
       </c>
     </row>
     <row r="3">
@@ -489,19 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40.41439637257</v>
+        <v>43.63070991305</v>
       </c>
       <c r="C3" t="n">
-        <v>101.28443555217</v>
+        <v>110.11073297724</v>
       </c>
       <c r="D3" t="n">
-        <v>91.59420005419</v>
+        <v>99.17654561585</v>
       </c>
       <c r="E3" t="n">
-        <v>3375.726404072921</v>
+        <v>4772.494032335781</v>
       </c>
       <c r="F3" t="n">
-        <v>16713.50206906343</v>
+        <v>24908.75805290864</v>
       </c>
     </row>
     <row r="4">
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>47.91023611345999</v>
+        <v>47.09307318523</v>
       </c>
       <c r="C4" t="n">
-        <v>78.03147630963001</v>
+        <v>78.00284813434999</v>
       </c>
       <c r="D4" t="n">
-        <v>49.14027593698</v>
+        <v>47.94975442803</v>
       </c>
       <c r="E4" t="n">
-        <v>4339.4083419977</v>
+        <v>4365.34005233962</v>
       </c>
       <c r="F4" t="n">
-        <v>5190.44496490223</v>
+        <v>5246.26399374735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>